<commit_message>
Time series plot: 4/14/2024
</commit_message>
<xml_diff>
--- a/data/ClearingEfficiency_v1.xlsx
+++ b/data/ClearingEfficiency_v1.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4f5e485ed766aa2/Pictures/Documents/Journal Publications/Manuscripts/Dissertation/CH2_Pomacea-Time-Series/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="272" documentId="8_{4A7C03E4-2DE5-493D-AB26-E395D3C5EFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77CBF1F7-D105-4D65-BEF4-39F65F746A97}"/>
+  <xr:revisionPtr revIDLastSave="277" documentId="8_{4A7C03E4-2DE5-493D-AB26-E395D3C5EFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0ECC5169-C999-40CB-8E1A-55CFE42CFA28}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FB82C6CD-E98C-47E6-ACFD-ED4329931F98}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="2" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -183,6 +187,18 @@
   </si>
   <si>
     <t>Checked.by</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of Y</t>
   </si>
 </sst>
 </file>
@@ -224,9 +240,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -244,8 +265,298 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Nathan Barrus" refreshedDate="45267.55617708333" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="73" xr:uid="{F12148DC-C839-4A50-9EDA-56112D3E8A27}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="J2:J75" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="1">
+    <cacheField name="Y" numFmtId="0">
+      <sharedItems containsBlank="1" count="3">
+        <s v="Y"/>
+        <s v="N"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="73">
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3239ECA8-6759-4FF0-8D37-94D6BAAC9A79}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Y" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -544,12 +855,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{089162EC-776D-4D66-A37B-4D662F899E9B}">
+  <dimension ref="A3:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="4">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192451DE-12CA-44E4-867F-93EA6DA62EBC}">
   <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P26" sqref="P26"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J75" sqref="J2:J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
1/2/2025 - Apple Snail Density Work
</commit_message>
<xml_diff>
--- a/data/ClearingEfficiency_v1.xlsx
+++ b/data/ClearingEfficiency_v1.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4f5e485ed766aa2/Pictures/Documents/Journal Publications/Manuscripts/Dissertation/CH2_Pomacea-Time-Series/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4f5e485ed766aa2/Pictures/Documents/Career/Journal Publications/Manuscripts/Dissertation/CH2_Pomacea-Time-Series/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="277" documentId="8_{4A7C03E4-2DE5-493D-AB26-E395D3C5EFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0ECC5169-C999-40CB-8E1A-55CFE42CFA28}"/>
+  <xr:revisionPtr revIDLastSave="278" documentId="8_{4A7C03E4-2DE5-493D-AB26-E395D3C5EFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{705F0EE8-53AF-43E1-A1A7-2FBBD34114A0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FB82C6CD-E98C-47E6-ACFD-ED4329931F98}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{FB82C6CD-E98C-47E6-ACFD-ED4329931F98}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId3"/>
-  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -187,18 +183,6 @@
   </si>
   <si>
     <t>Checked.by</t>
-  </si>
-  <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
-    <t>(blank)</t>
-  </si>
-  <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
-    <t>Count of Y</t>
   </si>
 </sst>
 </file>
@@ -240,14 +224,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -265,304 +244,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Nathan Barrus" refreshedDate="45267.55617708333" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="73" xr:uid="{F12148DC-C839-4A50-9EDA-56112D3E8A27}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="J2:J75" sheet="Sheet1"/>
-  </cacheSource>
-  <cacheFields count="1">
-    <cacheField name="Y" numFmtId="0">
-      <sharedItems containsBlank="1" count="3">
-        <s v="Y"/>
-        <s v="N"/>
-        <m/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="73">
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3239ECA8-6759-4FF0-8D37-94D6BAAC9A79}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="1">
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Y" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -600,7 +285,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -706,7 +391,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -848,74 +533,17 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{089162EC-776D-4D66-A37B-4D662F899E9B}">
-  <dimension ref="A3:B7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="4">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="4">
-        <v>71</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192451DE-12CA-44E4-867F-93EA6DA62EBC}">
   <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J75" sqref="J2:J75"/>
     </sheetView>

</xml_diff>